<commit_message>
Add period + separate deductions
</commit_message>
<xml_diff>
--- a/DataEntryFormSample/PayrollCalculator_template.xlsx
+++ b/DataEntryFormSample/PayrollCalculator_template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\DataEntryFormSample\DataEntryFormSample\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4BAB9FF-DCD9-4F5F-980E-31D0030788B1}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98A50663-03D9-4135-8E0F-8A926873805E}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{73FB3FD1-26D8-4C14-9D27-733BB681B0DF}"/>
   </bookViews>
@@ -110,7 +110,7 @@
     <numFmt numFmtId="164" formatCode="_([$$-409]* #,##0.00_);_([$$-409]* \(#,##0.00\);_([$$-409]* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="165" formatCode="#0;;;"/>
   </numFmts>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -149,6 +149,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1" tint="0.249977111117893"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="4">
@@ -199,7 +205,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -223,10 +229,16 @@
       <alignment horizontal="right" vertical="center" indent="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="1" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="10" fontId="1" fillId="3" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="10" fontId="2" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -547,391 +559,352 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1C78F302-F8E0-4241-BC15-D1E925132DAD}">
-  <dimension ref="B1:L25"/>
+  <dimension ref="B1:J25"/>
   <sheetViews>
     <sheetView showGridLines="0" showRowColHeaders="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="5.7109375" customWidth="1"/>
     <col min="2" max="2" width="3.28515625" customWidth="1"/>
-    <col min="6" max="6" width="24.7109375" customWidth="1"/>
-    <col min="7" max="7" width="3.7109375" customWidth="1"/>
-    <col min="8" max="8" width="3.42578125" customWidth="1"/>
-    <col min="9" max="9" width="3.5703125" customWidth="1"/>
-    <col min="10" max="10" width="29.5703125" customWidth="1"/>
-    <col min="11" max="11" width="19.7109375" customWidth="1"/>
-    <col min="12" max="12" width="3.7109375" customWidth="1"/>
+    <col min="3" max="3" width="29.7109375" customWidth="1"/>
+    <col min="4" max="4" width="24.7109375" customWidth="1"/>
+    <col min="5" max="5" width="3.7109375" customWidth="1"/>
+    <col min="6" max="6" width="3.42578125" customWidth="1"/>
+    <col min="7" max="7" width="3.5703125" customWidth="1"/>
+    <col min="8" max="8" width="29.5703125" customWidth="1"/>
+    <col min="9" max="9" width="19.7109375" customWidth="1"/>
+    <col min="10" max="10" width="3.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:12" ht="42.75" customHeight="1" x14ac:dyDescent="0.65">
-      <c r="B1" s="11" t="s">
+    <row r="1" spans="2:10" ht="42.75" customHeight="1" x14ac:dyDescent="0.65">
+      <c r="B1" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="11"/>
-      <c r="D1" s="11"/>
-      <c r="E1" s="11"/>
-      <c r="F1" s="11"/>
-      <c r="G1" s="11"/>
-    </row>
-    <row r="3" spans="2:12" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C1" s="15"/>
+      <c r="D1" s="15"/>
+      <c r="E1" s="15"/>
+      <c r="J1" s="14" t="str">
+        <f ca="1">CONCATENATE("Period: ",TEXT(NOW(), "M/d/yyyy"))</f>
+        <v>Period: 7/31/2019</v>
+      </c>
+    </row>
+    <row r="3" spans="2:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B3" s="3"/>
       <c r="C3" s="3"/>
       <c r="D3" s="3"/>
       <c r="E3" s="3"/>
-      <c r="F3" s="3"/>
       <c r="G3" s="3"/>
+      <c r="H3" s="3"/>
       <c r="I3" s="3"/>
       <c r="J3" s="3"/>
-      <c r="K3" s="3"/>
-      <c r="L3" s="3"/>
-    </row>
-    <row r="4" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="4" spans="2:10" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B4" s="3"/>
       <c r="C4" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="D4" s="3"/>
-      <c r="E4" s="3"/>
-      <c r="F4" s="2" t="s">
+      <c r="D4" s="16" t="s">
         <v>11</v>
       </c>
-      <c r="G4" s="1"/>
-      <c r="I4" s="3"/>
-      <c r="J4" s="3" t="s">
+      <c r="E4" s="1"/>
+      <c r="G4" s="3"/>
+      <c r="H4" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="K4" s="3">
+      <c r="I4" s="3">
         <v>1</v>
       </c>
-      <c r="L4" s="3"/>
-    </row>
-    <row r="5" spans="2:12" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="J4" s="3"/>
+    </row>
+    <row r="5" spans="2:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B5" s="3"/>
       <c r="C5" s="3"/>
       <c r="D5" s="3"/>
       <c r="E5" s="3"/>
-      <c r="F5" s="3"/>
       <c r="G5" s="3"/>
+      <c r="H5" s="3"/>
       <c r="I5" s="3"/>
       <c r="J5" s="3"/>
-      <c r="K5" s="3"/>
-      <c r="L5" s="3"/>
-    </row>
-    <row r="6" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="6" spans="2:10" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B6" s="3"/>
       <c r="C6" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="D6" s="3"/>
+      <c r="D6" s="5">
+        <v>10</v>
+      </c>
       <c r="E6" s="3"/>
-      <c r="F6" s="5">
-        <v>10</v>
-      </c>
       <c r="G6" s="3"/>
-      <c r="I6" s="3"/>
-      <c r="J6" s="3" t="s">
+      <c r="H6" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="K6" s="3">
+      <c r="I6" s="3">
         <v>4</v>
       </c>
-      <c r="L6" s="3"/>
-    </row>
-    <row r="7" spans="2:12" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="J6" s="3"/>
+    </row>
+    <row r="7" spans="2:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B7" s="3"/>
       <c r="C7" s="3"/>
       <c r="D7" s="3"/>
       <c r="E7" s="3"/>
-      <c r="F7" s="3"/>
       <c r="G7" s="3"/>
+      <c r="H7" s="3"/>
       <c r="I7" s="3"/>
       <c r="J7" s="3"/>
-      <c r="K7" s="3"/>
-      <c r="L7" s="3"/>
-    </row>
-    <row r="8" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="8" spans="2:10" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B8" s="3"/>
       <c r="C8" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="D8" s="3"/>
+      <c r="D8" s="8">
+        <v>40</v>
+      </c>
       <c r="E8" s="3"/>
-      <c r="F8" s="8">
-        <v>40</v>
-      </c>
       <c r="G8" s="3"/>
-      <c r="I8" s="3"/>
-      <c r="J8" s="3" t="s">
+      <c r="H8" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="K8" s="13">
+      <c r="I8" s="12">
         <v>2.3E-2</v>
       </c>
-      <c r="L8" s="3"/>
-    </row>
-    <row r="9" spans="2:12" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="J8" s="3"/>
+    </row>
+    <row r="9" spans="2:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B9" s="3"/>
       <c r="C9" s="3"/>
       <c r="D9" s="3"/>
       <c r="E9" s="3"/>
-      <c r="F9" s="3"/>
       <c r="G9" s="3"/>
+      <c r="H9" s="3"/>
       <c r="I9" s="3"/>
       <c r="J9" s="3"/>
-      <c r="K9" s="3"/>
-      <c r="L9" s="3"/>
-    </row>
-    <row r="10" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="10" spans="2:10" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B10" s="3"/>
       <c r="C10" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D10" s="3"/>
+      <c r="D10" s="8">
+        <v>5</v>
+      </c>
       <c r="E10" s="3"/>
-      <c r="F10" s="8">
-        <v>5</v>
-      </c>
       <c r="G10" s="3"/>
-      <c r="I10" s="3"/>
-      <c r="J10" s="3" t="s">
+      <c r="H10" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="K10" s="13">
+      <c r="I10" s="12">
         <v>0.28000000000000003</v>
       </c>
-      <c r="L10" s="3"/>
-    </row>
-    <row r="11" spans="2:12" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="J10" s="3"/>
+    </row>
+    <row r="11" spans="2:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B11" s="3"/>
       <c r="C11" s="3"/>
       <c r="D11" s="3"/>
       <c r="E11" s="3"/>
-      <c r="F11" s="3"/>
       <c r="G11" s="3"/>
+      <c r="H11" s="3"/>
       <c r="I11" s="3"/>
       <c r="J11" s="3"/>
-      <c r="K11" s="3"/>
-      <c r="L11" s="3"/>
-    </row>
-    <row r="12" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="12" spans="2:10" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B12" s="3"/>
       <c r="C12" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="D12" s="3"/>
+      <c r="D12" s="9">
+        <v>1</v>
+      </c>
       <c r="E12" s="3"/>
-      <c r="F12" s="9">
-        <v>1</v>
-      </c>
       <c r="G12" s="3"/>
-      <c r="I12" s="3"/>
-      <c r="J12" s="3" t="s">
+      <c r="H12" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="K12" s="13">
+      <c r="I12" s="12">
         <v>6.3E-2</v>
       </c>
-      <c r="L12" s="3"/>
-    </row>
-    <row r="13" spans="2:12" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="J12" s="3"/>
+    </row>
+    <row r="13" spans="2:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B13" s="3"/>
       <c r="C13" s="3"/>
       <c r="D13" s="3"/>
       <c r="E13" s="3"/>
-      <c r="F13" s="3"/>
       <c r="G13" s="3"/>
+      <c r="H13" s="3"/>
       <c r="I13" s="3"/>
       <c r="J13" s="3"/>
-      <c r="K13" s="3"/>
-      <c r="L13" s="3"/>
-    </row>
-    <row r="14" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="14" spans="2:10" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B14" s="3"/>
       <c r="C14" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="D14" s="3"/>
+      <c r="D14" s="8"/>
       <c r="E14" s="3"/>
-      <c r="F14" s="8"/>
       <c r="G14" s="3"/>
-      <c r="I14" s="3"/>
-      <c r="J14" s="3" t="s">
+      <c r="H14" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="K14" s="13">
+      <c r="I14" s="12">
         <v>1.4500000000000001E-2</v>
       </c>
-      <c r="L14" s="3"/>
-    </row>
-    <row r="15" spans="2:12" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="J14" s="3"/>
+    </row>
+    <row r="15" spans="2:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B15" s="3"/>
       <c r="C15" s="3"/>
       <c r="D15" s="3"/>
       <c r="E15" s="3"/>
-      <c r="F15" s="3"/>
       <c r="G15" s="3"/>
+      <c r="H15" s="3"/>
       <c r="I15" s="3"/>
       <c r="J15" s="3"/>
-      <c r="K15" s="3"/>
-      <c r="L15" s="3"/>
-    </row>
-    <row r="16" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="16" spans="2:10" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B16" s="3"/>
       <c r="C16" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="D16" s="3"/>
+      <c r="D16" s="10"/>
       <c r="E16" s="3"/>
-      <c r="F16" s="10"/>
       <c r="G16" s="3"/>
-      <c r="I16" s="3"/>
-      <c r="J16" s="2" t="s">
+      <c r="H16" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="K16" s="14">
-        <f>SUM(K8,K10,K12,K14)</f>
+      <c r="I16" s="13">
+        <f>SUM(I8,I10,I12,I14)</f>
         <v>0.38050000000000006</v>
       </c>
-      <c r="L16" s="3"/>
-    </row>
-    <row r="17" spans="2:12" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="J16" s="3"/>
+    </row>
+    <row r="17" spans="2:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B17" s="3"/>
       <c r="C17" s="3"/>
       <c r="D17" s="3"/>
       <c r="E17" s="3"/>
-      <c r="F17" s="3"/>
       <c r="G17" s="3"/>
+      <c r="H17" s="3"/>
       <c r="I17" s="3"/>
       <c r="J17" s="3"/>
-      <c r="K17" s="3"/>
-      <c r="L17" s="3"/>
-    </row>
-    <row r="18" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="18" spans="2:10" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B18" s="3"/>
       <c r="C18" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D18" s="3"/>
+      <c r="D18" s="5">
+        <f>D6*(D8+D10+D12)+D14*D16</f>
+        <v>460</v>
+      </c>
       <c r="E18" s="3"/>
-      <c r="F18" s="5">
-        <f>F6*(F8+F10+F12)+F14*F16</f>
-        <v>460</v>
-      </c>
-      <c r="G18" s="3"/>
-      <c r="I18" s="3"/>
-      <c r="J18" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="K18" s="12">
-        <v>20</v>
-      </c>
-      <c r="L18" s="3"/>
-    </row>
-    <row r="19" spans="2:12" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="19" spans="2:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B19" s="3"/>
       <c r="C19" s="3"/>
       <c r="D19" s="3"/>
       <c r="E19" s="3"/>
-      <c r="F19" s="3"/>
       <c r="G19" s="3"/>
+      <c r="H19" s="3"/>
       <c r="I19" s="3"/>
       <c r="J19" s="3"/>
-      <c r="K19" s="3"/>
-      <c r="L19" s="3"/>
-    </row>
-    <row r="20" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="20" spans="2:10" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B20" s="3"/>
       <c r="C20" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D20" s="3"/>
+      <c r="D20" s="5">
+        <f>D18*I16+I24</f>
+        <v>235.03000000000003</v>
+      </c>
       <c r="E20" s="3"/>
-      <c r="F20" s="5">
-        <f>F18*K16+K22</f>
-        <v>235.03000000000003</v>
-      </c>
       <c r="G20" s="3"/>
-      <c r="I20" s="3"/>
-      <c r="J20" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="K20" s="12">
-        <v>40</v>
-      </c>
-      <c r="L20" s="3"/>
-    </row>
-    <row r="21" spans="2:12" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="H20" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="I20" s="11">
+        <v>20</v>
+      </c>
+      <c r="J20" s="3"/>
+    </row>
+    <row r="21" spans="2:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B21" s="3"/>
       <c r="C21" s="3"/>
       <c r="D21" s="3"/>
       <c r="E21" s="3"/>
-      <c r="F21" s="3"/>
       <c r="G21" s="3"/>
+      <c r="H21" s="3"/>
       <c r="I21" s="3"/>
       <c r="J21" s="3"/>
-      <c r="K21" s="3"/>
-      <c r="L21" s="3"/>
-    </row>
-    <row r="22" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="22" spans="2:10" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B22" s="3"/>
       <c r="C22" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="D22" s="3"/>
+      <c r="D22" s="4">
+        <v>20</v>
+      </c>
       <c r="E22" s="3"/>
-      <c r="F22" s="4">
-        <v>20</v>
-      </c>
       <c r="G22" s="3"/>
-      <c r="I22" s="3"/>
-      <c r="J22" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="K22" s="5">
-        <f>SUM(K18,K20)</f>
-        <v>60</v>
-      </c>
-      <c r="L22" s="3"/>
-    </row>
-    <row r="23" spans="2:12" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="H22" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="I22" s="11">
+        <v>40</v>
+      </c>
+      <c r="J22" s="3"/>
+    </row>
+    <row r="23" spans="2:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B23" s="3"/>
       <c r="C23" s="3"/>
       <c r="D23" s="3"/>
       <c r="E23" s="3"/>
-      <c r="F23" s="3"/>
       <c r="G23" s="3"/>
+      <c r="H23" s="3"/>
       <c r="I23" s="3"/>
       <c r="J23" s="3"/>
-      <c r="K23" s="3"/>
-      <c r="L23" s="3"/>
-    </row>
-    <row r="24" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="24" spans="2:10" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B24" s="3"/>
       <c r="C24" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="D24" s="3"/>
+      <c r="D24" s="7">
+        <f>D18-D20-D22</f>
+        <v>204.96999999999997</v>
+      </c>
       <c r="E24" s="3"/>
-      <c r="F24" s="7">
-        <f>F18-F20-F22</f>
-        <v>204.96999999999997</v>
-      </c>
       <c r="G24" s="3"/>
-    </row>
-    <row r="25" spans="2:12" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="H24" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="I24" s="5">
+        <f>SUM(I20,I22)</f>
+        <v>60</v>
+      </c>
+      <c r="J24" s="3"/>
+    </row>
+    <row r="25" spans="2:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B25" s="3"/>
       <c r="C25" s="3"/>
       <c r="D25" s="3"/>
       <c r="E25" s="3"/>
-      <c r="F25" s="3"/>
       <c r="G25" s="3"/>
+      <c r="H25" s="3"/>
+      <c r="I25" s="3"/>
+      <c r="J25" s="3"/>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="B1:G1"/>
+    <mergeCell ref="B1:E1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
Refactoring + number formats
</commit_message>
<xml_diff>
--- a/DataEntryFormSample/PayrollCalculator_template.xlsx
+++ b/DataEntryFormSample/PayrollCalculator_template.xlsx
@@ -8,10 +8,10 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\DataEntryFormSample\DataEntryFormSample\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5EC2AA74-1BA4-4D44-BCBE-2EE6D6D2BCEB}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{027A9D63-B0C8-46E0-9550-F1C7A7128C6F}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <workbookProtection workbookPassword="CF7A" lockStructure="1"/>
   <bookViews>
-    <workbookView xWindow="3765" yWindow="1230" windowWidth="17085" windowHeight="13245" xr2:uid="{73FB3FD1-26D8-4C14-9D27-733BB681B0DF}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{73FB3FD1-26D8-4C14-9D27-733BB681B0DF}"/>
   </bookViews>
   <sheets>
     <sheet name="Payroll Calculator" sheetId="1" r:id="rId1"/>
@@ -109,7 +109,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="_([$$-409]* #,##0.00_);_([$$-409]* \(#,##0.00\);_([$$-409]* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="165" formatCode="#0;;;"/>
+    <numFmt numFmtId="166" formatCode="#0_)"/>
   </numFmts>
   <fonts count="7" x14ac:knownFonts="1">
     <font>
@@ -206,7 +206,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -218,14 +218,6 @@
     <xf numFmtId="164" fontId="2" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="4" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right" vertical="center" indent="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="165" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right" vertical="center" indent="1"/>
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="164" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right" vertical="center" indent="1"/>
       <protection locked="0"/>
@@ -240,6 +232,10 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="166" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -581,15 +577,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:10" ht="42.75" customHeight="1" x14ac:dyDescent="0.65">
-      <c r="B1" s="16" t="s">
+      <c r="B1" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="16"/>
-      <c r="D1" s="16"/>
-      <c r="E1" s="16"/>
-      <c r="J1" s="14" t="str">
+      <c r="C1" s="14"/>
+      <c r="D1" s="14"/>
+      <c r="E1" s="14"/>
+      <c r="J1" s="12" t="str">
         <f ca="1">CONCATENATE("Period: ",TEXT(NOW(), "M/d/yyyy"))</f>
-        <v>Period: 7/31/2019</v>
+        <v>Period: 8/1/2019</v>
       </c>
     </row>
     <row r="3" spans="2:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
@@ -607,7 +603,7 @@
       <c r="C4" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="D4" s="15" t="s">
+      <c r="D4" s="13" t="s">
         <v>11</v>
       </c>
       <c r="E4" s="1"/>
@@ -663,7 +659,7 @@
       <c r="C8" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="D8" s="8">
+      <c r="D8" s="15">
         <v>40</v>
       </c>
       <c r="E8" s="3"/>
@@ -671,7 +667,7 @@
       <c r="H8" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="I8" s="12">
+      <c r="I8" s="10">
         <v>2.3E-2</v>
       </c>
       <c r="J8" s="3"/>
@@ -691,7 +687,7 @@
       <c r="C10" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D10" s="8">
+      <c r="D10" s="15">
         <v>5</v>
       </c>
       <c r="E10" s="3"/>
@@ -699,7 +695,7 @@
       <c r="H10" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="I10" s="12">
+      <c r="I10" s="10">
         <v>0.28000000000000003</v>
       </c>
       <c r="J10" s="3"/>
@@ -719,7 +715,7 @@
       <c r="C12" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="D12" s="9">
+      <c r="D12" s="15">
         <v>1</v>
       </c>
       <c r="E12" s="3"/>
@@ -727,7 +723,7 @@
       <c r="H12" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="I12" s="12">
+      <c r="I12" s="10">
         <v>6.3E-2</v>
       </c>
       <c r="J12" s="3"/>
@@ -747,13 +743,13 @@
       <c r="C14" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="D14" s="8"/>
+      <c r="D14" s="15"/>
       <c r="E14" s="3"/>
       <c r="G14" s="3"/>
       <c r="H14" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="I14" s="12">
+      <c r="I14" s="10">
         <v>1.4500000000000001E-2</v>
       </c>
       <c r="J14" s="3"/>
@@ -773,13 +769,13 @@
       <c r="C16" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="D16" s="10"/>
+      <c r="D16" s="8"/>
       <c r="E16" s="3"/>
       <c r="G16" s="3"/>
       <c r="H16" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="I16" s="13">
+      <c r="I16" s="11">
         <f>SUM(I8,I10,I12,I14)</f>
         <v>0.38050000000000006</v>
       </c>
@@ -830,7 +826,7 @@
       <c r="H20" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="I20" s="11">
+      <c r="I20" s="9">
         <v>20</v>
       </c>
       <c r="J20" s="3"/>
@@ -858,7 +854,7 @@
       <c r="H22" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="I22" s="11">
+      <c r="I22" s="9">
         <v>40</v>
       </c>
       <c r="J22" s="3"/>

</xml_diff>